<commit_message>
datasync: Update template columns names.
</commit_message>
<xml_diff>
--- a/co2mpas/datasync_template.xlsx
+++ b/co2mpas/datasync_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Time [s]</t>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>Theoretical Velocity [km/h]</t>
+  </si>
+  <si>
+    <t>Dyno Engine Speed [rpm]</t>
+  </si>
+  <si>
+    <t>Dyno Engine Coolant Temperature [oC]</t>
+  </si>
+  <si>
+    <t>Dyno Calculated Engine Load  [%]</t>
+  </si>
+  <si>
+    <t>OBD Gear  [-]</t>
+  </si>
+  <si>
+    <t>OBD CO2 [g/s]</t>
   </si>
 </sst>
 </file>
@@ -7616,7 +7631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1761"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7645,13 +7662,13 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -25358,7 +25375,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1753"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25384,7 +25403,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -25405,7 +25424,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>19</v>

</xml_diff>